<commit_message>
7/13 before the game
</commit_message>
<xml_diff>
--- a/Figures/eval.xlsx
+++ b/Figures/eval.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="30" windowWidth="28755" windowHeight="12840" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="30" windowWidth="28755" windowHeight="12840"/>
   </bookViews>
   <sheets>
     <sheet name="IPC" sheetId="1" r:id="rId1"/>
@@ -121,10 +121,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="167" formatCode="0.0000%"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -150,15 +158,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -279,11 +290,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="114685440"/>
-        <c:axId val="114686976"/>
+        <c:axId val="138999296"/>
+        <c:axId val="139000832"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="114685440"/>
+        <c:axId val="138999296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -305,7 +316,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="114686976"/>
+        <c:crossAx val="139000832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -313,7 +324,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="114686976"/>
+        <c:axId val="139000832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -359,7 +370,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="114685440"/>
+        <c:crossAx val="138999296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="2.0000000000000009E-3"/>
@@ -503,11 +514,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="116148864"/>
-        <c:axId val="116162944"/>
+        <c:axId val="139950720"/>
+        <c:axId val="139956608"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="116148864"/>
+        <c:axId val="139950720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -529,7 +540,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="116162944"/>
+        <c:crossAx val="139956608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -537,7 +548,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="116162944"/>
+        <c:axId val="139956608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.30000000000000004"/>
@@ -591,7 +602,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="116148864"/>
+        <c:crossAx val="139950720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1.0000000000000002E-2"/>
@@ -705,11 +716,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="116178944"/>
-        <c:axId val="116180480"/>
+        <c:axId val="139980800"/>
+        <c:axId val="139982336"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="116178944"/>
+        <c:axId val="139980800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -731,7 +742,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="116180480"/>
+        <c:crossAx val="139982336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -739,7 +750,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="116180480"/>
+        <c:axId val="139982336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -785,7 +796,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="116178944"/>
+        <c:crossAx val="139980800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="2.0000000000000005E-3"/>
@@ -922,11 +933,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="115956352"/>
-        <c:axId val="115958144"/>
+        <c:axId val="140600448"/>
+        <c:axId val="140601984"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="115956352"/>
+        <c:axId val="140600448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -948,7 +959,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="115958144"/>
+        <c:crossAx val="140601984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -956,7 +967,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="115958144"/>
+        <c:axId val="140601984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1002,7 +1013,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="115956352"/>
+        <c:crossAx val="140600448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="2.0000000000000005E-3"/>
@@ -1521,11 +1532,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="114"/>
-        <c:axId val="116016256"/>
-        <c:axId val="116017792"/>
+        <c:axId val="140657408"/>
+        <c:axId val="140658944"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="116016256"/>
+        <c:axId val="140657408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1534,7 +1545,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116017792"/>
+        <c:crossAx val="140658944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1542,7 +1553,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="116017792"/>
+        <c:axId val="140658944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="280"/>
@@ -1574,7 +1585,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116016256"/>
+        <c:crossAx val="140657408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1733,11 +1744,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="144379904"/>
-        <c:axId val="144381440"/>
+        <c:axId val="140683904"/>
+        <c:axId val="140702080"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="144379904"/>
+        <c:axId val="140683904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1756,7 +1767,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="144381440"/>
+        <c:crossAx val="140702080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1764,7 +1775,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="144381440"/>
+        <c:axId val="140702080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="70"/>
@@ -1805,7 +1816,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="144379904"/>
+        <c:crossAx val="140683904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2061,11 +2072,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="121589760"/>
-        <c:axId val="121592832"/>
+        <c:axId val="140267904"/>
+        <c:axId val="140270208"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="121589760"/>
+        <c:axId val="140267904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2110,7 +2121,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="121592832"/>
+        <c:crossAx val="140270208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2118,7 +2129,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="121592832"/>
+        <c:axId val="140270208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="80"/>
@@ -2165,7 +2176,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="121589760"/>
+        <c:crossAx val="140267904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2714,8 +2725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M33" sqref="M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2982,7 +2993,7 @@
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G22">
+      <c r="G22" s="2">
         <f>G20/B20</f>
         <v>0.99941981189690987</v>
       </c>
@@ -3017,7 +3028,7 @@
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B37">
+      <c r="B37" s="2">
         <f>B35/B33</f>
         <v>0.99851334951456316</v>
       </c>
@@ -3110,8 +3121,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="U52" sqref="U52"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J42" sqref="J42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3542,7 +3553,7 @@
         <v>24</v>
       </c>
       <c r="G27">
-        <f t="shared" ref="B27:G27" si="5">G17*G7</f>
+        <f t="shared" ref="G27" si="5">G17*G7</f>
         <v>73.243712000000002</v>
       </c>
       <c r="H27">
@@ -3555,7 +3566,7 @@
         <v>23</v>
       </c>
       <c r="G28">
-        <f t="shared" ref="B28:G28" si="6">G18*G8</f>
+        <f t="shared" ref="G28" si="6">G18*G8</f>
         <v>88.918870799999993</v>
       </c>
       <c r="H28">

</xml_diff>